<commit_message>
WIP MDT Pragma's toegevoegd. Versie demo Bob
</commit_message>
<xml_diff>
--- a/MDT/RollenEnBeheerdersPassen/Identiteiten_extra.xlsx
+++ b/MDT/RollenEnBeheerdersPassen/Identiteiten_extra.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20136" windowHeight="9516" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20136" windowHeight="9516" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Bevoegdheid" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="110">
   <si>
     <t>AL</t>
   </si>
@@ -223,9 +223,6 @@
     <t>Zakelijke Klant</t>
   </si>
   <si>
-    <t>[Bevoegdheid]</t>
-  </si>
-  <si>
     <t>[Certificaat]</t>
   </si>
   <si>
@@ -268,9 +265,6 @@
     <t>Beheerder_1</t>
   </si>
   <si>
-    <t>AutoX</t>
-  </si>
-  <si>
     <t>KlantRol_1</t>
   </si>
   <si>
@@ -292,9 +286,6 @@
     <t>Klant_2</t>
   </si>
   <si>
-    <t>LeaseY</t>
-  </si>
-  <si>
     <t>Verkoop</t>
   </si>
   <si>
@@ -308,6 +299,60 @@
   </si>
   <si>
     <t>Schade</t>
+  </si>
+  <si>
+    <t>Bevoegdheid]</t>
+  </si>
+  <si>
+    <t>[Beheerder]</t>
+  </si>
+  <si>
+    <t>Auto X</t>
+  </si>
+  <si>
+    <t>Leasemaatschap Y</t>
+  </si>
+  <si>
+    <t>[KlantRol]</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>c3</t>
+  </si>
+  <si>
+    <t>c4</t>
+  </si>
+  <si>
+    <t>c5</t>
+  </si>
+  <si>
+    <t>c6</t>
+  </si>
+  <si>
+    <t>c7</t>
+  </si>
+  <si>
+    <t>c8</t>
+  </si>
+  <si>
+    <t>c9</t>
+  </si>
+  <si>
+    <t>geautoriseerd</t>
+  </si>
+  <si>
+    <t>1008</t>
+  </si>
+  <si>
+    <t>1003</t>
+  </si>
+  <si>
+    <t>8888</t>
   </si>
 </sst>
 </file>
@@ -343,8 +388,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -633,13 +680,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
         <v>77</v>
-      </c>
-      <c r="C1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -946,18 +993,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -966,6 +1018,78 @@
       </c>
       <c r="B2" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -975,258 +1099,180 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>68</v>
       </c>
       <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="D22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>79</v>
       </c>
-      <c r="B3" t="str">
-        <f t="shared" ref="B3:D11" si="0">IF(ISERROR(SEARCH(B$1&amp;"_",$A3,1)),"",$A3)</f>
-        <v>Klant_1</v>
-      </c>
-      <c r="C3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D4" t="str">
-        <f t="shared" si="0"/>
-        <v>Beheerder_1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>KlantRol_1</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B6" t="str">
-        <f>IF(ISERROR(SEARCH(B$1&amp;"_",$A6,1)),"",$A6)</f>
-        <v/>
-      </c>
-      <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v>KlantRol_2</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" ref="B7:D11" si="1">IF(ISERROR(SEARCH(B$1&amp;"_",$A7,1)),"",$A7)</f>
-        <v/>
-      </c>
-      <c r="C7" t="str">
-        <f t="shared" si="0"/>
-        <v>KlantRol_3</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>85</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C8" t="str">
-        <f t="shared" si="0"/>
-        <v>KlantRol_4</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E8" t="s">
-        <v>88</v>
-      </c>
-      <c r="G8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>86</v>
-      </c>
-      <c r="B9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C9" t="str">
-        <f t="shared" si="0"/>
-        <v>KlantRol_5</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E9" t="s">
-        <v>88</v>
-      </c>
-      <c r="G9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v>Beheerder_2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" t="str">
-        <f t="shared" si="1"/>
-        <v>Klant_2</v>
-      </c>
-      <c r="C11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F11" t="s">
-        <v>87</v>
-      </c>
-      <c r="G11" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1240,10 +1286,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1261,20 +1307,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1287,7 +1333,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -1295,7 +1341,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
         <v>57</v>
@@ -1303,10 +1349,50 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP MDT afsprakendocument v0.3
</commit_message>
<xml_diff>
--- a/MDT/RollenEnBeheerdersPassen/Identiteiten_extra.xlsx
+++ b/MDT/RollenEnBeheerdersPassen/Identiteiten_extra.xlsx
@@ -9,21 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20136" windowHeight="9516" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20136" windowHeight="9516" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Bevoegdheid" sheetId="1" r:id="rId1"/>
     <sheet name="Certificaat" sheetId="2" r:id="rId2"/>
     <sheet name="Identiteit" sheetId="3" r:id="rId3"/>
-    <sheet name="gekoppeldAan" sheetId="6" r:id="rId4"/>
-    <sheet name="heeft" sheetId="7" r:id="rId5"/>
+    <sheet name="heeft" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="108">
   <si>
     <t>AL</t>
   </si>
@@ -229,13 +228,7 @@
     <t>[Klant]</t>
   </si>
   <si>
-    <t>[ProcID]</t>
-  </si>
-  <si>
     <t>beheerder</t>
-  </si>
-  <si>
-    <t>gekoppeldAan</t>
   </si>
   <si>
     <t>heeft</t>
@@ -680,13 +673,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1009,7 +1002,7 @@
         <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1022,74 +1015,74 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1116,13 +1109,13 @@
         <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1138,38 +1131,38 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1185,71 +1178,71 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" t="s">
         <v>83</v>
       </c>
-      <c r="B18" t="s">
-        <v>85</v>
-      </c>
       <c r="D18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1262,12 +1255,12 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1278,40 +1271,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1322,7 +1284,7 @@
         <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1335,7 +1297,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -1343,7 +1305,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
         <v>56</v>
@@ -1351,7 +1313,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -1362,7 +1324,7 @@
         <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1370,31 +1332,31 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nieuwe info van Jan Willem verwerkt
</commit_message>
<xml_diff>
--- a/MDT/RollenEnBeheerdersPassen/Identiteiten_extra.xlsx
+++ b/MDT/RollenEnBeheerdersPassen/Identiteiten_extra.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20136" windowHeight="9516" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20136" windowHeight="9516" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bevoegdheid" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="117">
   <si>
     <t>AL</t>
   </si>
@@ -255,97 +255,124 @@
     <t>Beheerder_1</t>
   </si>
   <si>
-    <t>KlantRol_1</t>
-  </si>
-  <si>
-    <t>KlantRol_2</t>
-  </si>
-  <si>
-    <t>KlantRol_3</t>
-  </si>
-  <si>
-    <t>KlantRol_4</t>
-  </si>
-  <si>
-    <t>KlantRol_5</t>
-  </si>
-  <si>
     <t>Beheerder_2</t>
   </si>
   <si>
     <t>Klant_2</t>
   </si>
   <si>
-    <t>Verkoop</t>
-  </si>
-  <si>
-    <t>Werkplaats</t>
-  </si>
-  <si>
-    <t>Directeur Piet</t>
-  </si>
-  <si>
-    <t>Onderhoud</t>
-  </si>
-  <si>
-    <t>Schade</t>
-  </si>
-  <si>
     <t>Bevoegdheid]</t>
   </si>
   <si>
     <t>[Beheerder]</t>
   </si>
   <si>
-    <t>Auto X</t>
-  </si>
-  <si>
-    <t>Leasemaatschap Y</t>
-  </si>
-  <si>
     <t>[KlantRol]</t>
   </si>
   <si>
-    <t>c1</t>
-  </si>
-  <si>
-    <t>c2</t>
-  </si>
-  <si>
-    <t>c3</t>
-  </si>
-  <si>
-    <t>c4</t>
-  </si>
-  <si>
-    <t>c5</t>
-  </si>
-  <si>
-    <t>c6</t>
-  </si>
-  <si>
-    <t>c7</t>
-  </si>
-  <si>
-    <t>c8</t>
-  </si>
-  <si>
-    <t>c9</t>
-  </si>
-  <si>
     <t>geautoriseerd</t>
   </si>
   <si>
-    <t>1008</t>
-  </si>
-  <si>
-    <t>1003</t>
-  </si>
-  <si>
     <t>8888</t>
   </si>
   <si>
     <t>ProcIdent</t>
+  </si>
+  <si>
+    <t>[Bevoegdheid;]</t>
+  </si>
+  <si>
+    <t>Klant_3</t>
+  </si>
+  <si>
+    <t>Klant_4</t>
+  </si>
+  <si>
+    <t>Klant_5</t>
+  </si>
+  <si>
+    <t>Klant_6</t>
+  </si>
+  <si>
+    <t>Beheerder_3</t>
+  </si>
+  <si>
+    <t>Beheerder_4</t>
+  </si>
+  <si>
+    <t>Beheerder_5</t>
+  </si>
+  <si>
+    <t>Beheerder_6</t>
+  </si>
+  <si>
+    <t>Garagebedrijf `de sleutelaar`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leasebedrijf Betabet </t>
+  </si>
+  <si>
+    <t>Garagebedrijf `de importeur`</t>
+  </si>
+  <si>
+    <t>De Exporteur B.V.</t>
+  </si>
+  <si>
+    <t>Sloopbedrijf `De moker`</t>
+  </si>
+  <si>
+    <t>Kentekenloket de balie</t>
+  </si>
+  <si>
+    <t>BV;TV</t>
+  </si>
+  <si>
+    <t>BV;TV;VA</t>
+  </si>
+  <si>
+    <t>BV;TV;VN</t>
+  </si>
+  <si>
+    <t>BV;EX</t>
+  </si>
+  <si>
+    <t>BV;DM</t>
+  </si>
+  <si>
+    <t>Certificaat_1</t>
+  </si>
+  <si>
+    <t>Certificaat_2</t>
+  </si>
+  <si>
+    <t>Certificaat_3</t>
+  </si>
+  <si>
+    <t>Certificaat_4</t>
+  </si>
+  <si>
+    <t>Certificaat_5</t>
+  </si>
+  <si>
+    <t>Certificaat_6</t>
+  </si>
+  <si>
+    <t>Certificaat_7</t>
+  </si>
+  <si>
+    <t>Certificaat_8</t>
+  </si>
+  <si>
+    <t>Certificaat_9</t>
+  </si>
+  <si>
+    <t>Certificaat_10</t>
+  </si>
+  <si>
+    <t>Certificaat_11</t>
+  </si>
+  <si>
+    <t>Certificaat_12</t>
   </si>
 </sst>
 </file>
@@ -673,7 +700,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B1" t="s">
         <v>73</v>
@@ -986,14 +1013,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1015,7 +1043,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
         <v>76</v>
@@ -1023,66 +1051,90 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1095,13 +1147,14 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23:D24"/>
+      <selection activeCell="A14" sqref="A14:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1137,23 +1190,67 @@
         <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" t="s">
         <v>92</v>
+      </c>
+      <c r="D7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B12" t="s">
         <v>71</v>
@@ -1176,64 +1273,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" t="s">
-        <v>87</v>
-      </c>
-    </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B21" t="s">
         <v>71</v>
@@ -1260,7 +1302,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1271,13 +1313,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1292,7 +1337,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1300,63 +1345,68 @@
         <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>105</v>
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>106</v>
+      <c r="B13" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>